<commit_message>
Consulta Apellido Solis en pagina cnt
</commit_message>
<xml_diff>
--- a/ContactosApellido.xlsx
+++ b/ContactosApellido.xlsx
@@ -34,7 +34,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+  <x:si>
+    <x:t>72280017</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAMPOVERDE SOLIS EDGAR MARCELO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RIO BOMBOISA Y RIO ESMERALDAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SEVILLA DE ORO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72280020</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAMPOVERDE SOLIS EDISSON GEOVANNY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RIOS EMERALDAS Y 21 DE AGOSTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72280096</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARDENAS SOLIS GLORIA NARCISA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SIMON BOLIVAR 0S Y 24 DE MAYO CASA BLOQUE CASA-BLOQUE SIMON BOLIVAR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72280223</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OLGA MERCEDES SOLIS LOPEZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SECTOR LA UNION</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72280051</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOLIS TAPIA MIGUEL ALBERTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DANIEL ARDENAS Y CRISTOBAL COLON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72280236</x:t>
+  </x:si>
+  <x:si>
+    <x:t>VILLAVICENCIO SOLIS JUAN GUALBERTO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SECTOR LA UNION 0 Y CHORDELEG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72271102</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHAVEZ SOLIS JUAN CARLOS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JOSE PERALTA 0 Y Y ABDON CALDERON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SANTA ISABEL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73011944</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOLIS CRESPO ELVIA EDID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TOMEBAMBA - NASTE 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PAUTE</x:t>
+  </x:si>
   <x:si>
     <x:t>Número Telefónico</x:t>
   </x:si>
@@ -48,7 +129,76 @@
     <x:t>Localidad</x:t>
   </x:si>
   <x:si>
-    <x:t>:: No hay teléfonos con estos datos ::</x:t>
+    <x:t>73051027</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ARMANDO VICENTE FLORES SOLIS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SECTOR NEGAS 0 KM6 VIA GUALACEO - CUENCA KM6 VIA GUALACEO - CUENCA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GUALACEO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73067044</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FLORES SOLIS RUTH MARIA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LLAMPASAY 0 CASA CREMA DE 1 PISO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73052952</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INGA SOLIS JOSEFINA DEL CARMEN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CARMEN DE BULLCAY 0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73011278</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INGA SOLIS RUTH CECILIA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BULLCAY 0 LAS ISLAS LAS ISLAS</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72282342</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MORA SOLIS ALCIDES FERNANDO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAN FRANCISCO 0 Y CENTRO CANTONAL CASA DE 2 PLANTAS COLOR CREMA CASA NUEVA CASA DE 2 PLANTAS COLOR CREMA CASA NUEVA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EL PAN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72282221</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SOLIS MOLINA ROSA BELLA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAN FRANCISCO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>72223950</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BLANCA CARMELA SOLIS LAGUATASIG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AV. 15 DE ABRIL 1 Y TEODORO WOLF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHORDELEG</x:t>
   </x:si>
   <x:si>
     <x:t>:: DATOS TELEFONICOS ::</x:t>
@@ -410,7 +560,7 @@
       <x:selection activeCell="E8" sqref="E8 E8:E8"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="114.335469" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="115.756719" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="22.710938" style="3" bestFit="1" customWidth="1"/>
     <x:col min="2" max="3" width="14.140625" style="3" customWidth="1"/>
@@ -437,13 +587,13 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C2" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D2" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E2" s="4">
         <x:f>COUNTA(D2:D1000)</x:f>
@@ -451,117 +601,229 @@
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A3" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B3" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D3" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E3" s="4">
         <x:f>COUNTIF(D2:D1000,"Localidad")</x:f>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="3" t="s"/>
-      <x:c r="B4" s="3" t="s"/>
-      <x:c r="C4" s="3" t="s"/>
-      <x:c r="D4" s="3" t="s"/>
+      <x:c r="A4" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
       <x:c r="E4" s="4">
         <x:f>COUNTIF(D2:D1000,":: DATOS TELEFONICOS ::")</x:f>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="3" t="s"/>
-      <x:c r="B5" s="3" t="s"/>
-      <x:c r="C5" s="3" t="s"/>
-      <x:c r="D5" s="3" t="s"/>
+      <x:c r="A5" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B5" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C5" s="3" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D5" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
       <x:c r="E5" s="4">
         <x:f>COUNTIF(D2:D1000,":: No hay teléfonos con estos datos ::")</x:f>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="3" t="s"/>
-      <x:c r="B6" s="3" t="s"/>
-      <x:c r="C6" s="3" t="s"/>
-      <x:c r="D6" s="3" t="s"/>
+      <x:c r="A6" s="3" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B6" s="3" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C6" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D6" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
       <x:c r="E6" s="4" t="s"/>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="3" t="s"/>
-      <x:c r="B7" s="3" t="s"/>
-      <x:c r="C7" s="3" t="s"/>
-      <x:c r="D7" s="3" t="s"/>
+      <x:c r="A7" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B7" s="3" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C7" s="3" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D7" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
       <x:c r="E7" s="4">
         <x:f>E2-E4-E5-E3</x:f>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="3" t="s"/>
-      <x:c r="B8" s="3" t="s"/>
-      <x:c r="C8" s="3" t="s"/>
-      <x:c r="D8" s="3" t="s"/>
+      <x:c r="A8" s="3" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B8" s="3" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C8" s="3" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="D8" s="3" t="s">
+        <x:v>26</x:v>
+      </x:c>
       <x:c r="E8" s="4" t="str">
         <x:f>IF(E7&lt;=1,"No existen contactos","Numero de contactos :"&amp;E7)</x:f>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
-      <x:c r="A9" s="3" t="s"/>
-      <x:c r="B9" s="3" t="s"/>
-      <x:c r="C9" s="3" t="s"/>
-      <x:c r="D9" s="3" t="s"/>
+      <x:c r="A9" s="3" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B9" s="3" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C9" s="3" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D9" s="3" t="s">
+        <x:v>30</x:v>
+      </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
-      <x:c r="A10" s="3" t="s"/>
-      <x:c r="B10" s="3" t="s"/>
-      <x:c r="C10" s="3" t="s"/>
-      <x:c r="D10" s="3" t="s"/>
+      <x:c r="A10" s="3" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B10" s="3" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C10" s="3" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="D10" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
-      <x:c r="A11" s="3" t="s"/>
-      <x:c r="B11" s="3" t="s"/>
-      <x:c r="C11" s="3" t="s"/>
-      <x:c r="D11" s="3" t="s"/>
+      <x:c r="A11" s="3" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B11" s="3" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C11" s="3" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D11" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
-      <x:c r="A12" s="3" t="s"/>
-      <x:c r="B12" s="3" t="s"/>
-      <x:c r="C12" s="3" t="s"/>
-      <x:c r="D12" s="3" t="s"/>
+      <x:c r="A12" s="3" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B12" s="3" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C12" s="3" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D12" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
-      <x:c r="A13" s="3" t="s"/>
-      <x:c r="B13" s="3" t="s"/>
-      <x:c r="C13" s="3" t="s"/>
-      <x:c r="D13" s="3" t="s"/>
+      <x:c r="A13" s="3" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B13" s="3" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C13" s="3" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="D13" s="3" t="s">
+        <x:v>34</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
-      <x:c r="A14" s="3" t="s"/>
-      <x:c r="B14" s="3" t="s"/>
-      <x:c r="C14" s="3" t="s"/>
-      <x:c r="D14" s="3" t="s"/>
+      <x:c r="A14" s="3" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B14" s="3" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C14" s="3" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D14" s="3" t="s">
+        <x:v>47</x:v>
+      </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
-      <x:c r="A15" s="3" t="s"/>
-      <x:c r="B15" s="3" t="s"/>
-      <x:c r="C15" s="3" t="s"/>
-      <x:c r="D15" s="3" t="s"/>
+      <x:c r="A15" s="3" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B15" s="3" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C15" s="3" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D15" s="3" t="s">
+        <x:v>47</x:v>
+      </x:c>
     </x:row>
     <x:row r="16" spans="1:5">
-      <x:c r="A16" s="3" t="s"/>
-      <x:c r="B16" s="3" t="s"/>
-      <x:c r="C16" s="3" t="s"/>
-      <x:c r="D16" s="3" t="s"/>
+      <x:c r="A16" s="3" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B16" s="3" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C16" s="3" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="D16" s="3" t="s">
+        <x:v>54</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="1:5">
-      <x:c r="A17" s="3" t="s"/>
-      <x:c r="B17" s="3" t="s"/>
-      <x:c r="C17" s="3" t="s"/>
-      <x:c r="D17" s="3" t="s"/>
+      <x:c r="A17" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B17" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C17" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D17" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="3" t="s"/>

</xml_diff>